<commit_message>
mbox network delay notes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balladaniel\Desktop\phd_local\pub_webmaps_codecomplexity_performance\webmaplibs_performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B16A82-3161-4D5C-A3D6-7C82EC4BFAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A06EF-CB2F-4CA3-AC17-1FADFA7999D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Polygons" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="30">
   <si>
     <t>Leaflet</t>
   </si>
@@ -119,12 +118,24 @@
   <si>
     <t>Polygons</t>
   </si>
+  <si>
+    <t>MBoxGLJS 1 db feature betolteset, sot, reteg nelkuli betolteset is kb 200msig csinalja, ugyhogy megiscsak network dolog. Plusz felfedezes: az mellett, hogy mar map object initnel kell lennie tokennek, ha elrontom a tokent (tehat van string, de rossz), akkor egy pillanatig megjelenik a terkep a pontommal, es utana eltuntet mindent.</t>
+  </si>
+  <si>
+    <t>Egy dolgot nem magyaraznak ezek: MLibGLJS miert hasonloan lassu?! Lehet csak veletlen a hasonlosag, es ennyit tud a MLib, tul van bonyolitva a kod es egyszeruen sokaig tart meg ugy is, hogy nincs semmi network request.</t>
+  </si>
+  <si>
+    <t>https://docs.mapbox.com/help/troubleshooting/working-with-large-geojson-data/</t>
+  </si>
+  <si>
+    <t>Konkluzio fele: mapbox kb 50000 featuretol veri le idoben a Leafletet es OL-t, csak azert mert tokent checkel/authol, ami megkerulhetetlen. Szep....</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +178,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -194,10 +213,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -207,8 +229,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -262,7 +293,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="sk-SK"/>
-              <a:t>Full chart: 50 - 500000 features</a:t>
+              <a:t>Full chart: 50 - 500000 features (LINEAR Y)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -1818,7 +1849,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="sk-SK"/>
-              <a:t>Full chart: 50 - 500000 features</a:t>
+              <a:t>Full chart: 50 - 500000 features (LOG Y)</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -1879,7 +1910,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Lines!$B$58:$J$58</c:f>
+              <c:f>Points!$B$58:$J$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1915,36 +1946,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Lines!$B$15:$J$15</c:f>
+              <c:f>Points!$B$15:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>19.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>32.166666666666664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>136.33333333333334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>245.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>962</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1993.6666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>10820</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1952,7 +1983,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CA50-4931-8A8C-D20D9044E140}"/>
+              <c16:uniqueId val="{00000000-7B51-49B0-84FD-FA5686FBC1E8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1976,7 +2007,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Lines!$B$58:$J$58</c:f>
+              <c:f>Points!$B$58:$J$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2012,36 +2043,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Lines!$B$33:$J$33</c:f>
+              <c:f>Points!$B$33:$J$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>258</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>268.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>310.33333333333331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>377.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>444</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>817</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1287</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>6530</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2049,7 +2080,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CA50-4931-8A8C-D20D9044E140}"/>
+              <c16:uniqueId val="{00000001-7B51-49B0-84FD-FA5686FBC1E8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2073,7 +2104,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Lines!$B$58:$J$58</c:f>
+              <c:f>Points!$B$58:$J$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2109,36 +2140,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Lines!$B$51:$J$51</c:f>
+              <c:f>Points!$B$51:$J$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>377.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>372</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>386.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>497</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1404.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2414</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>12395</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2146,7 +2177,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-CA50-4931-8A8C-D20D9044E140}"/>
+              <c16:uniqueId val="{00000002-7B51-49B0-84FD-FA5686FBC1E8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2170,7 +2201,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Lines!$B$58:$J$58</c:f>
+              <c:f>Points!$B$58:$J$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -2206,36 +2237,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Lines!$B$69:$J$69</c:f>
+              <c:f>Points!$B$69:$J$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>30.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>30.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>727.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1373</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>7205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2243,7 +2274,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-CA50-4931-8A8C-D20D9044E140}"/>
+              <c16:uniqueId val="{00000003-7B51-49B0-84FD-FA5686FBC1E8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2369,6 +2400,7 @@
       <c:valAx>
         <c:axId val="445001359"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2604,7 +2636,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="sk-SK"/>
-              <a:t>Excerpt for 50 - 10000 features</a:t>
+              <a:t>Full chart: 50 - 500000 features</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -2665,17 +2697,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Lines!$B$58:$J$58</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Lines!$B$58:$G$58</c:f>
+              <c:f>Lines!$B$58:$J$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -2693,23 +2718,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Lines!$B$15:$J$15</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Lines!$B$15:$G$15</c:f>
+              <c:f>Lines!$B$15:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2726,6 +2753,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2734,7 +2770,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8456-456C-A35C-5BE0499180A6}"/>
+              <c16:uniqueId val="{00000000-CA50-4931-8A8C-D20D9044E140}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2758,17 +2794,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Lines!$B$58:$J$58</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Lines!$B$58:$G$58</c:f>
+              <c:f>Lines!$B$58:$J$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -2786,23 +2815,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Lines!$B$33:$J$33</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Lines!$B$33:$G$33</c:f>
+              <c:f>Lines!$B$33:$J$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2819,6 +2850,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2827,7 +2867,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8456-456C-A35C-5BE0499180A6}"/>
+              <c16:uniqueId val="{00000001-CA50-4931-8A8C-D20D9044E140}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2851,17 +2891,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Lines!$B$58:$J$58</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Lines!$B$58:$G$58</c:f>
+              <c:f>Lines!$B$58:$J$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -2879,23 +2912,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Lines!$B$51:$J$51</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Lines!$B$51:$G$51</c:f>
+              <c:f>Lines!$B$51:$J$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2912,6 +2947,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2920,7 +2964,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8456-456C-A35C-5BE0499180A6}"/>
+              <c16:uniqueId val="{00000002-CA50-4931-8A8C-D20D9044E140}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2944,17 +2988,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Lines!$B$58:$J$58</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Lines!$B$58:$G$58</c:f>
+              <c:f>Lines!$B$58:$J$58</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -2972,23 +3009,25 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Lines!$B$69:$J$69</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Lines!$B$69:$G$69</c:f>
+              <c:f>Lines!$B$69:$J$69</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3005,6 +3044,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3013,7 +3061,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8456-456C-A35C-5BE0499180A6}"/>
+              <c16:uniqueId val="{00000003-CA50-4931-8A8C-D20D9044E140}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3374,6 +3422,776 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="sk-SK"/>
+              <a:t>Excerpt for 50 - 10000 features</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Leaflet</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Lines!$B$58:$J$58</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Lines!$B$58:$G$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Lines!$B$15:$J$15</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Lines!$B$15:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8456-456C-A35C-5BE0499180A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MBoxGLJS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Lines!$B$58:$J$58</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Lines!$B$58:$G$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Lines!$B$33:$J$33</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Lines!$B$33:$G$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8456-456C-A35C-5BE0499180A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>MLibGLJS</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Lines!$B$58:$J$58</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Lines!$B$58:$G$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Lines!$B$51:$J$51</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Lines!$B$51:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8456-456C-A35C-5BE0499180A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>OpenLayers</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Lines!$B$58:$J$58</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Lines!$B$58:$G$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Lines!$B$69:$J$69</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Lines!$B$69:$G$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-8456-456C-A35C-5BE0499180A6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="444999919"/>
+        <c:axId val="445001359"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="444999919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sk-SK"/>
+                  <a:t>Feature count</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="445001359"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="445001359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sk-SK"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6405667412378821E-2"/>
+              <c:y val="0.42257846817365263"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="444999919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK"/>
               <a:t>Full chart: 50 - 500000 features</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
@@ -4125,7 +4943,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -5135,6 +5953,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -7716,6 +8574,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8272,15 +9646,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8302,6 +9676,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>147638</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFCCA9B0-DF93-4C52-AF97-C51DA11062A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8735,10 +10147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U71"/>
+  <dimension ref="A1:AB71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8747,10 +10159,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8767,17 +10179,17 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="U3" t="s">
         <v>12</v>
       </c>
@@ -8883,16 +10295,16 @@
       <c r="J6">
         <v>10530</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
       <c r="U6" t="s">
         <v>15</v>
       </c>
@@ -8919,14 +10331,14 @@
       <c r="I7">
         <v>1993</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
       <c r="U7" t="s">
         <v>16</v>
       </c>
@@ -8944,14 +10356,14 @@
       <c r="D8">
         <v>33</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
       <c r="U8" t="s">
         <v>17</v>
       </c>
@@ -8966,14 +10378,14 @@
       <c r="D9">
         <v>29</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -9151,19 +10563,22 @@
       <c r="C20" t="s">
         <v>3</v>
       </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -9219,13 +10634,13 @@
       <c r="G23" s="2">
         <v>444</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="11">
         <v>817</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="11">
         <v>1287</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="11">
         <v>6530</v>
       </c>
     </row>
@@ -9248,6 +10663,7 @@
       <c r="F24" s="2">
         <v>385</v>
       </c>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -9260,6 +10676,7 @@
         <v>317</v>
       </c>
       <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -9270,6 +10687,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -9280,6 +10698,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -9290,6 +10709,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
@@ -9300,6 +10720,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -9310,6 +10731,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -9320,6 +10742,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -9330,8 +10753,9 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -9372,7 +10796,7 @@
         <v>6530</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -9412,8 +10836,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L34" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -9453,32 +10880,60 @@
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L36" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L35" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="U35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="V35" s="9"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="9"/>
+      <c r="Y35" s="9"/>
+      <c r="Z35" s="9"/>
+      <c r="AA35" s="9"/>
+    </row>
+    <row r="36" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L36" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="9"/>
+      <c r="W36" s="9"/>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="9"/>
+      <c r="Z36" s="9"/>
+      <c r="AA36" s="9"/>
+      <c r="AB36" s="8"/>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="12"/>
+      <c r="R37" s="12"/>
+      <c r="S37" s="12"/>
+      <c r="T37" s="12"/>
+      <c r="U37" s="9"/>
+      <c r="V37" s="9"/>
+      <c r="W37" s="9"/>
+      <c r="X37" s="9"/>
+      <c r="Y37" s="9"/>
+      <c r="Z37" s="9"/>
+      <c r="AA37" s="9"/>
+      <c r="AB37" s="8"/>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -9488,24 +10943,57 @@
       <c r="C38" t="s">
         <v>3</v>
       </c>
-      <c r="L38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
+      <c r="L38" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="9"/>
+      <c r="Y38" s="9"/>
+      <c r="Z38" s="9"/>
+      <c r="AA38" s="9"/>
+      <c r="AB38" s="8"/>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="9"/>
+      <c r="X39" s="9"/>
+      <c r="Y39" s="9"/>
+      <c r="Z39" s="9"/>
+      <c r="AA39" s="9"/>
+      <c r="AB39" s="8"/>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
@@ -9536,8 +11024,17 @@
       <c r="J40" s="1">
         <v>500000</v>
       </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -9569,7 +11066,7 @@
         <v>12440</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -9601,7 +11098,7 @@
         <v>12350</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -9612,7 +11109,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>4</v>
       </c>
@@ -9620,22 +11117,22 @@
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>8</v>
       </c>
@@ -9785,17 +11282,17 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -10066,14 +11563,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="L6:S9"/>
+    <mergeCell ref="L36:T37"/>
+    <mergeCell ref="U35:AA39"/>
+    <mergeCell ref="L38:T40"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B39:J39"/>
     <mergeCell ref="B57:J57"/>
-    <mergeCell ref="L6:S9"/>
-    <mergeCell ref="L36:T37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10095,10 +11594,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -10115,17 +11614,17 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="U3" t="s">
         <v>12</v>
       </c>
@@ -10177,16 +11676,16 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
       <c r="U6" t="s">
         <v>15</v>
       </c>
@@ -10195,14 +11694,14 @@
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
       <c r="U7" t="s">
         <v>16</v>
       </c>
@@ -10211,14 +11710,14 @@
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
       <c r="U8" t="s">
         <v>17</v>
       </c>
@@ -10227,14 +11726,14 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -10396,17 +11895,17 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -10668,28 +12167,28 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L36" s="5" t="s">
+      <c r="L36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -10706,17 +12205,17 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -10935,17 +12434,17 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -11182,11 +12681,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -11203,17 +12702,17 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
       <c r="U3" t="s">
         <v>12</v>
       </c>
@@ -11265,16 +12764,16 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
       <c r="U6" t="s">
         <v>15</v>
       </c>
@@ -11283,14 +12782,14 @@
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
       <c r="U7" t="s">
         <v>16</v>
       </c>
@@ -11299,14 +12798,14 @@
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
       <c r="U8" t="s">
         <v>17</v>
       </c>
@@ -11315,14 +12814,14 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -11484,17 +12983,17 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -11756,28 +13255,28 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L36" s="5" t="s">
+      <c r="L36" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -11794,17 +13293,17 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -12023,17 +13522,17 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">

</xml_diff>

<commit_message>
3070 pc - points to check perf vs. igpu
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balladaniel\Desktop\phd_local\pub_webmaps_codecomplexity_performance\webmaplibs_performance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdnl\Desktop\phd_local\pub_webmaps_codecomplexity_performance\webmaplibs_performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A06EF-CB2F-4CA3-AC17-1FADFA7999D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D81BF0-4518-4CCC-ACE0-618EA99BA9CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Points" sheetId="1" r:id="rId1"/>
-    <sheet name="Lines" sheetId="4" r:id="rId2"/>
-    <sheet name="Polygons" sheetId="5" r:id="rId3"/>
+    <sheet name="Points_AFTERBURN_PC" sheetId="6" r:id="rId2"/>
+    <sheet name="Lines" sheetId="4" r:id="rId3"/>
+    <sheet name="Polygons" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="32">
   <si>
     <t>Leaflet</t>
   </si>
@@ -130,12 +131,18 @@
   <si>
     <t>Konkluzio fele: mapbox kb 50000 featuretol veri le idoben a Leafletet es OL-t, csak azert mert tokent checkel/authol, ami megkerulhetetlen. Szep....</t>
   </si>
+  <si>
+    <t>just to see if having a strong GPU makes a difference in non-opengl and opengl libraries</t>
+  </si>
+  <si>
+    <t>PC WITH 3070 (OPENGL!) / R5 3600</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +193,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -213,34 +228,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,7 +277,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1047,7 +1063,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1817,7 +1833,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2604,7 +2620,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3390,7 +3406,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4160,7 +4176,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4946,7 +4962,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10149,8 +10165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10159,10 +10175,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -10179,17 +10195,17 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
       <c r="U3" t="s">
         <v>12</v>
       </c>
@@ -10295,16 +10311,16 @@
       <c r="J6">
         <v>10530</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
       <c r="U6" t="s">
         <v>15</v>
       </c>
@@ -10331,14 +10347,14 @@
       <c r="I7">
         <v>1993</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
       <c r="U7" t="s">
         <v>16</v>
       </c>
@@ -10356,14 +10372,14 @@
       <c r="D8">
         <v>33</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
       <c r="U8" t="s">
         <v>17</v>
       </c>
@@ -10378,14 +10394,14 @@
       <c r="D9">
         <v>29</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -10568,17 +10584,17 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -10634,13 +10650,13 @@
       <c r="G23" s="2">
         <v>444</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23">
         <v>817</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23">
         <v>1287</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23">
         <v>6530</v>
       </c>
     </row>
@@ -10836,7 +10852,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L34" s="10" t="s">
+      <c r="L34" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -10880,58 +10896,58 @@
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L35" s="7" t="s">
+      <c r="L35" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U35" s="9" t="s">
+      <c r="U35" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="V35" s="9"/>
-      <c r="W35" s="9"/>
-      <c r="X35" s="9"/>
-      <c r="Y35" s="9"/>
-      <c r="Z35" s="9"/>
-      <c r="AA35" s="9"/>
+      <c r="V35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="X35" s="8"/>
+      <c r="Y35" s="8"/>
+      <c r="Z35" s="8"/>
+      <c r="AA35" s="8"/>
     </row>
     <row r="36" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L36" s="12" t="s">
+      <c r="L36" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-      <c r="R36" s="12"/>
-      <c r="S36" s="12"/>
-      <c r="T36" s="12"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
-      <c r="W36" s="9"/>
-      <c r="X36" s="9"/>
-      <c r="Y36" s="9"/>
-      <c r="Z36" s="9"/>
-      <c r="AA36" s="9"/>
-      <c r="AB36" s="8"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="8"/>
+      <c r="V36" s="8"/>
+      <c r="W36" s="8"/>
+      <c r="X36" s="8"/>
+      <c r="Y36" s="8"/>
+      <c r="Z36" s="8"/>
+      <c r="AA36" s="8"/>
+      <c r="AB36" s="4"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="12"/>
-      <c r="S37" s="12"/>
-      <c r="T37" s="12"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="9"/>
-      <c r="W37" s="9"/>
-      <c r="X37" s="9"/>
-      <c r="Y37" s="9"/>
-      <c r="Z37" s="9"/>
-      <c r="AA37" s="9"/>
-      <c r="AB37" s="8"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="8"/>
+      <c r="V37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="X37" s="8"/>
+      <c r="Y37" s="8"/>
+      <c r="Z37" s="8"/>
+      <c r="AA37" s="8"/>
+      <c r="AB37" s="4"/>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -10943,55 +10959,55 @@
       <c r="C38" t="s">
         <v>3</v>
       </c>
-      <c r="L38" s="9" t="s">
+      <c r="L38" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="9"/>
-      <c r="U38" s="9"/>
-      <c r="V38" s="9"/>
-      <c r="W38" s="9"/>
-      <c r="X38" s="9"/>
-      <c r="Y38" s="9"/>
-      <c r="Z38" s="9"/>
-      <c r="AA38" s="9"/>
-      <c r="AB38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
+      <c r="V38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="8"/>
+      <c r="Y38" s="8"/>
+      <c r="Z38" s="8"/>
+      <c r="AA38" s="8"/>
+      <c r="AB38" s="4"/>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
-      <c r="U39" s="9"/>
-      <c r="V39" s="9"/>
-      <c r="W39" s="9"/>
-      <c r="X39" s="9"/>
-      <c r="Y39" s="9"/>
-      <c r="Z39" s="9"/>
-      <c r="AA39" s="9"/>
-      <c r="AB39" s="8"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
+      <c r="V39" s="8"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="8"/>
+      <c r="Y39" s="8"/>
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="8"/>
+      <c r="AB39" s="4"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -11024,15 +11040,15 @@
       <c r="J40" s="1">
         <v>500000</v>
       </c>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
-      <c r="T40" s="9"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41">
@@ -11282,17 +11298,17 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -11564,6 +11580,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B57:J57"/>
     <mergeCell ref="L6:S9"/>
     <mergeCell ref="L36:T37"/>
     <mergeCell ref="U35:AA39"/>
@@ -11572,7 +11589,6 @@
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="B39:J39"/>
-    <mergeCell ref="B57:J57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11581,6 +11597,1301 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7326F72D-FE2E-4499-9C3F-B7DCE9FC1F96}">
+  <dimension ref="A1:M71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K61" sqref="K61"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="D1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1">
+        <v>500</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="I4" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J4" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>102</v>
+      </c>
+      <c r="G5">
+        <v>198</v>
+      </c>
+      <c r="H5">
+        <v>820</v>
+      </c>
+      <c r="I5">
+        <v>1569</v>
+      </c>
+      <c r="J5">
+        <v>11060</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>41</v>
+      </c>
+      <c r="F6">
+        <v>104</v>
+      </c>
+      <c r="G6">
+        <v>185</v>
+      </c>
+      <c r="H6">
+        <v>807</v>
+      </c>
+      <c r="I6">
+        <v>1578</v>
+      </c>
+      <c r="J6">
+        <v>11300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>35</v>
+      </c>
+      <c r="F7">
+        <v>105</v>
+      </c>
+      <c r="G7">
+        <v>191</v>
+      </c>
+      <c r="H7">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>103</v>
+      </c>
+      <c r="G8">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <f>AVERAGE(B5:B14)</f>
+        <v>12.25</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" ref="C15:J15" si="0">AVERAGE(C5:C14)</f>
+        <v>14.5</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>25.25</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="0"/>
+        <v>36.4</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="0"/>
+        <v>103.5</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>190</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>817</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="0"/>
+        <v>1573.5</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="0"/>
+        <v>11180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <f>_xlfn.STDEV.P(B5:B14)</f>
+        <v>0.82915619758884995</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:I16" si="1">_xlfn.STDEV.P(C5:C14)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>0.4330127018922193</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>2.3323807579381204</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>1.1180339887498949</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>5.1478150704935004</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>7.2571803523590805</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="J16">
+        <f>_xlfn.STDEV.P(J5:J14)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <f>_xlfn.STDEV.S(B5:B14)</f>
+        <v>0.9574271077563381</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:J17" si="2">_xlfn.STDEV.S(C5:C14)</f>
+        <v>0.57735026918962573</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>2.6076809620810599</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>1.2909944487358056</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>5.9441848333756697</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>8.8881944173155887</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>6.3639610306789276</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>169.70562748477141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1">
+        <v>50</v>
+      </c>
+      <c r="C22" s="1">
+        <v>100</v>
+      </c>
+      <c r="D22" s="1">
+        <v>500</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F22" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G22" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H22" s="1">
+        <v>50000</v>
+      </c>
+      <c r="I22" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J22" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="13">
+        <v>140</v>
+      </c>
+      <c r="C23" s="13">
+        <v>135</v>
+      </c>
+      <c r="D23" s="13">
+        <v>144</v>
+      </c>
+      <c r="E23" s="13">
+        <v>150</v>
+      </c>
+      <c r="F23" s="13">
+        <v>185</v>
+      </c>
+      <c r="G23" s="13">
+        <v>224</v>
+      </c>
+      <c r="H23" s="13">
+        <v>456</v>
+      </c>
+      <c r="I23" s="13">
+        <v>715</v>
+      </c>
+      <c r="J23" s="13">
+        <v>4253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13">
+        <v>136</v>
+      </c>
+      <c r="D24" s="13">
+        <v>140</v>
+      </c>
+      <c r="E24" s="13">
+        <v>153</v>
+      </c>
+      <c r="F24" s="13">
+        <v>194</v>
+      </c>
+      <c r="G24" s="13">
+        <v>228</v>
+      </c>
+      <c r="H24" s="13">
+        <v>451</v>
+      </c>
+      <c r="I24" s="13">
+        <v>809</v>
+      </c>
+      <c r="J24" s="13">
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13">
+        <v>139</v>
+      </c>
+      <c r="E25" s="13">
+        <v>149</v>
+      </c>
+      <c r="F25" s="13">
+        <v>185</v>
+      </c>
+      <c r="G25" s="13">
+        <v>234</v>
+      </c>
+      <c r="J25" s="13">
+        <v>3821</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" ref="B33:J33" si="3">AVERAGE(B23:B32)</f>
+        <v>140</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="3"/>
+        <v>135.5</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="3"/>
+        <v>141</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="3"/>
+        <v>150.66666666666666</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+      <c r="G33" s="1">
+        <f>AVERAGE(G23:G32)</f>
+        <v>228.66666666666666</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="3"/>
+        <v>453.5</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="3"/>
+        <v>762</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="3"/>
+        <v>4054.6666666666665</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ref="B34:J34" si="4">_xlfn.STDEV.P(B23:B32)</f>
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="4"/>
+        <v>2.1602468994692869</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="4"/>
+        <v>1.699673171197595</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="4"/>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="G34">
+        <f>_xlfn.STDEV.P(G23:G32)</f>
+        <v>4.1096093353126513</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="4"/>
+        <v>178.12417641135136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="e">
+        <f t="shared" ref="B35:J35" si="5">_xlfn.STDEV.S(B23:B32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="5"/>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="5"/>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="5"/>
+        <v>2.0816659994661331</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="5"/>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="G35">
+        <f>_xlfn.STDEV.S(G23:G32)</f>
+        <v>5.0332229568471671</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="5"/>
+        <v>3.5355339059327378</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="5"/>
+        <v>66.468037431535464</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="5"/>
+        <v>218.15667153065323</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1">
+        <v>50</v>
+      </c>
+      <c r="C40" s="1">
+        <v>100</v>
+      </c>
+      <c r="D40" s="1">
+        <v>500</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F40" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G40" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H40" s="1">
+        <v>50000</v>
+      </c>
+      <c r="I40" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J40" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>353</v>
+      </c>
+      <c r="C41">
+        <v>355</v>
+      </c>
+      <c r="D41">
+        <v>350</v>
+      </c>
+      <c r="E41">
+        <v>357</v>
+      </c>
+      <c r="F41">
+        <v>353</v>
+      </c>
+      <c r="G41">
+        <v>352</v>
+      </c>
+      <c r="H41">
+        <v>1060</v>
+      </c>
+      <c r="I41">
+        <v>1907</v>
+      </c>
+      <c r="J41">
+        <v>10590</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>353</v>
+      </c>
+      <c r="C42">
+        <v>354</v>
+      </c>
+      <c r="D42">
+        <v>352</v>
+      </c>
+      <c r="E42">
+        <v>348</v>
+      </c>
+      <c r="F42">
+        <v>356</v>
+      </c>
+      <c r="G42">
+        <v>363</v>
+      </c>
+      <c r="H42">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>351</v>
+      </c>
+      <c r="C43">
+        <v>350</v>
+      </c>
+      <c r="D43">
+        <v>353</v>
+      </c>
+      <c r="E43">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="E44">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="1">
+        <f>AVERAGE(B41:B50)</f>
+        <v>352.33333333333331</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" ref="C51:J51" si="6">AVERAGE(C41:C50)</f>
+        <v>353</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="6"/>
+        <v>351.66666666666669</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="6"/>
+        <v>351.5</v>
+      </c>
+      <c r="F51" s="1">
+        <f t="shared" si="6"/>
+        <v>354.5</v>
+      </c>
+      <c r="G51" s="1">
+        <f t="shared" si="6"/>
+        <v>357.5</v>
+      </c>
+      <c r="H51" s="1">
+        <f t="shared" si="6"/>
+        <v>1050.5</v>
+      </c>
+      <c r="I51" s="1">
+        <f t="shared" si="6"/>
+        <v>1907</v>
+      </c>
+      <c r="J51" s="1">
+        <f t="shared" si="6"/>
+        <v>10590</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <f>_xlfn.STDEV.P(B41:B50)</f>
+        <v>0.94280904158206336</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ref="C52:J52" si="7">_xlfn.STDEV.P(C41:C50)</f>
+        <v>2.1602468994692869</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="7"/>
+        <v>1.247219128924647</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="7"/>
+        <v>3.7749172176353749</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="7"/>
+        <v>5.5</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="7"/>
+        <v>9.5</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53">
+        <f>_xlfn.STDEV.S(B41:B50)</f>
+        <v>1.1547005383792517</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ref="C53:J53" si="8">_xlfn.STDEV.S(C41:C50)</f>
+        <v>2.6457513110645907</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="8"/>
+        <v>1.5275252316519465</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="8"/>
+        <v>4.358898943540674</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="8"/>
+        <v>2.1213203435596424</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="8"/>
+        <v>7.7781745930520225</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="8"/>
+        <v>13.435028842544403</v>
+      </c>
+      <c r="I53" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J53" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="1">
+        <v>50</v>
+      </c>
+      <c r="C58" s="1">
+        <v>100</v>
+      </c>
+      <c r="D58" s="1">
+        <v>500</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F58" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G58" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H58" s="1">
+        <v>50000</v>
+      </c>
+      <c r="I58" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J58" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>30</v>
+      </c>
+      <c r="C59">
+        <v>34</v>
+      </c>
+      <c r="D59">
+        <v>42</v>
+      </c>
+      <c r="E59">
+        <v>54</v>
+      </c>
+      <c r="F59">
+        <v>101</v>
+      </c>
+      <c r="G59">
+        <v>158</v>
+      </c>
+      <c r="H59">
+        <v>526</v>
+      </c>
+      <c r="I59">
+        <v>1052</v>
+      </c>
+      <c r="J59">
+        <v>5893</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2</v>
+      </c>
+      <c r="B60">
+        <v>29</v>
+      </c>
+      <c r="C60">
+        <v>32</v>
+      </c>
+      <c r="D60">
+        <v>42</v>
+      </c>
+      <c r="E60">
+        <v>57</v>
+      </c>
+      <c r="F60">
+        <v>106</v>
+      </c>
+      <c r="G60">
+        <v>158</v>
+      </c>
+      <c r="H60">
+        <v>537</v>
+      </c>
+      <c r="I60">
+        <v>1071</v>
+      </c>
+      <c r="J60">
+        <v>5920</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>30</v>
+      </c>
+      <c r="C61">
+        <v>32</v>
+      </c>
+      <c r="D61">
+        <v>42</v>
+      </c>
+      <c r="E61">
+        <v>53</v>
+      </c>
+      <c r="F61">
+        <v>106</v>
+      </c>
+      <c r="H61">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="1">
+        <f>AVERAGE(B59:B68)</f>
+        <v>29.666666666666668</v>
+      </c>
+      <c r="C69" s="1">
+        <f t="shared" ref="C69:J69" si="9">AVERAGE(C59:C68)</f>
+        <v>32.666666666666664</v>
+      </c>
+      <c r="D69" s="1">
+        <f>AVERAGE(D59:D68)</f>
+        <v>42</v>
+      </c>
+      <c r="E69" s="1">
+        <f t="shared" si="9"/>
+        <v>54.666666666666664</v>
+      </c>
+      <c r="F69" s="1">
+        <f t="shared" si="9"/>
+        <v>104.33333333333333</v>
+      </c>
+      <c r="G69" s="1">
+        <f t="shared" si="9"/>
+        <v>158</v>
+      </c>
+      <c r="H69" s="1">
+        <f t="shared" si="9"/>
+        <v>535.33333333333337</v>
+      </c>
+      <c r="I69" s="1">
+        <f t="shared" si="9"/>
+        <v>1061.5</v>
+      </c>
+      <c r="J69" s="1">
+        <f t="shared" si="9"/>
+        <v>5906.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70">
+        <f>_xlfn.STDEV.P(B59:B68)</f>
+        <v>0.47140452079103168</v>
+      </c>
+      <c r="C70">
+        <f t="shared" ref="C70:J70" si="10">_xlfn.STDEV.P(C59:C68)</f>
+        <v>0.94280904158206336</v>
+      </c>
+      <c r="D70">
+        <f>_xlfn.STDEV.P(D59:D68)</f>
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="10"/>
+        <v>1.699673171197595</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="10"/>
+        <v>2.3570226039551581</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="10"/>
+        <v>7.0395706939809592</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="10"/>
+        <v>9.5</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="10"/>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71">
+        <f>_xlfn.STDEV.S(B59:B68)</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="C71">
+        <f t="shared" ref="C71:J71" si="11">_xlfn.STDEV.S(C59:C68)</f>
+        <v>1.1547005383792517</v>
+      </c>
+      <c r="D71">
+        <f>_xlfn.STDEV.S(D59:D68)</f>
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="11"/>
+        <v>2.0816659994661326</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="11"/>
+        <v>2.8867513459481287</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="11"/>
+        <v>8.6216781042517088</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="11"/>
+        <v>13.435028842544403</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="11"/>
+        <v>19.091883092036785</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B57:J57"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0788AADB-FA8C-4ED4-A981-E1DCADC2505D}">
   <dimension ref="A1:U71"/>
   <sheetViews>
@@ -11594,10 +12905,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -11614,17 +12925,17 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
       <c r="U3" t="s">
         <v>12</v>
       </c>
@@ -11676,16 +12987,16 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
       <c r="U6" t="s">
         <v>15</v>
       </c>
@@ -11694,14 +13005,14 @@
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
       <c r="U7" t="s">
         <v>16</v>
       </c>
@@ -11710,14 +13021,14 @@
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
       <c r="U8" t="s">
         <v>17</v>
       </c>
@@ -11726,14 +13037,14 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -11895,17 +13206,17 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -12167,28 +13478,28 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L36" s="6" t="s">
+      <c r="L36" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -12205,17 +13516,17 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -12434,17 +13745,17 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
@@ -12667,7 +13978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08824990-74A8-40EE-8C04-5F1E3002B771}">
   <dimension ref="A1:U71"/>
   <sheetViews>
@@ -12681,11 +13992,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -12702,17 +14013,17 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
       <c r="U3" t="s">
         <v>12</v>
       </c>
@@ -12764,16 +14075,16 @@
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
       <c r="U6" t="s">
         <v>15</v>
       </c>
@@ -12782,14 +14093,14 @@
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
       <c r="U7" t="s">
         <v>16</v>
       </c>
@@ -12798,14 +14109,14 @@
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
       <c r="U8" t="s">
         <v>17</v>
       </c>
@@ -12814,14 +14125,14 @@
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -12983,17 +14294,17 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -13255,28 +14566,28 @@
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L36" s="6" t="s">
+      <c r="L36" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -13293,17 +14604,17 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -13522,17 +14833,17 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">

</xml_diff>

<commit_message>
cleanup, results.xls - dataset sizes
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\balladaniel\Desktop\phd_local\pub_webmaps_codecomplexity_performance\webmaplibs_performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E47FC53-E409-4FAF-A597-AB4976B092EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401FA170-A405-415F-AF09-2C6E46E35009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Points" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Lines_3070PC" sheetId="8" r:id="rId4"/>
     <sheet name="Polygons" sheetId="7" r:id="rId5"/>
     <sheet name="Polygons_3070PC" sheetId="9" r:id="rId6"/>
+    <sheet name="DatasetFileSizes" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="51">
   <si>
     <t>Run #</t>
   </si>
@@ -173,6 +174,27 @@
   </si>
   <si>
     <t>weak PC (iGPU, OpenGL 4.4)</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Number of features</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>lines</t>
+  </si>
+  <si>
+    <t>polygons</t>
+  </si>
+  <si>
+    <t>Filesizes</t>
+  </si>
+  <si>
+    <t>KB</t>
   </si>
 </sst>
 </file>
@@ -406,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,6 +466,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,19 +508,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -26332,34 +26360,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
-      <c r="L1" s="32" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
+      <c r="L1" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
@@ -26374,14 +26402,14 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
       <c r="U2" t="s">
         <v>32</v>
       </c>
@@ -26399,14 +26427,14 @@
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
       <c r="J3" s="22"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
       <c r="U3" t="s">
         <v>7</v>
       </c>
@@ -26445,14 +26473,14 @@
       <c r="J4" s="13">
         <v>500000</v>
       </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
       <c r="U4" t="s">
         <v>8</v>
       </c>
@@ -26940,10 +26968,10 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
         <v>6</v>
@@ -27285,61 +27313,61 @@
       <c r="L35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U35" s="34" t="s">
+      <c r="U35" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="V35" s="34"/>
-      <c r="W35" s="34"/>
-      <c r="X35" s="34"/>
-      <c r="Y35" s="34"/>
-      <c r="Z35" s="34"/>
-      <c r="AA35" s="34"/>
+      <c r="V35" s="25"/>
+      <c r="W35" s="25"/>
+      <c r="X35" s="25"/>
+      <c r="Y35" s="25"/>
+      <c r="Z35" s="25"/>
+      <c r="AA35" s="25"/>
     </row>
     <row r="36" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L36" s="33" t="s">
+      <c r="L36" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="M36" s="33"/>
-      <c r="N36" s="33"/>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="33"/>
-      <c r="R36" s="33"/>
-      <c r="S36" s="33"/>
-      <c r="T36" s="33"/>
-      <c r="U36" s="34"/>
-      <c r="V36" s="34"/>
-      <c r="W36" s="34"/>
-      <c r="X36" s="34"/>
-      <c r="Y36" s="34"/>
-      <c r="Z36" s="34"/>
-      <c r="AA36" s="34"/>
+      <c r="M36" s="24"/>
+      <c r="N36" s="24"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="24"/>
+      <c r="Q36" s="24"/>
+      <c r="R36" s="24"/>
+      <c r="S36" s="24"/>
+      <c r="T36" s="24"/>
+      <c r="U36" s="25"/>
+      <c r="V36" s="25"/>
+      <c r="W36" s="25"/>
+      <c r="X36" s="25"/>
+      <c r="Y36" s="25"/>
+      <c r="Z36" s="25"/>
+      <c r="AA36" s="25"/>
       <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-      <c r="N37" s="33"/>
-      <c r="O37" s="33"/>
-      <c r="P37" s="33"/>
-      <c r="Q37" s="33"/>
-      <c r="R37" s="33"/>
-      <c r="S37" s="33"/>
-      <c r="T37" s="33"/>
-      <c r="U37" s="34"/>
-      <c r="V37" s="34"/>
-      <c r="W37" s="34"/>
-      <c r="X37" s="34"/>
-      <c r="Y37" s="34"/>
-      <c r="Z37" s="34"/>
-      <c r="AA37" s="34"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="T37" s="24"/>
+      <c r="U37" s="25"/>
+      <c r="V37" s="25"/>
+      <c r="W37" s="25"/>
+      <c r="X37" s="25"/>
+      <c r="Y37" s="25"/>
+      <c r="Z37" s="25"/>
+      <c r="AA37" s="25"/>
       <c r="AB37" s="3"/>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="27"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="7" t="s">
         <v>6</v>
       </c>
@@ -27352,24 +27380,24 @@
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="8"/>
-      <c r="L38" s="34" t="s">
+      <c r="L38" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="34"/>
-      <c r="P38" s="34"/>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="34"/>
-      <c r="S38" s="34"/>
-      <c r="T38" s="34"/>
-      <c r="U38" s="34"/>
-      <c r="V38" s="34"/>
-      <c r="W38" s="34"/>
-      <c r="X38" s="34"/>
-      <c r="Y38" s="34"/>
-      <c r="Z38" s="34"/>
-      <c r="AA38" s="34"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="25"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="25"/>
+      <c r="Q38" s="25"/>
+      <c r="R38" s="25"/>
+      <c r="S38" s="25"/>
+      <c r="T38" s="25"/>
+      <c r="U38" s="25"/>
+      <c r="V38" s="25"/>
+      <c r="W38" s="25"/>
+      <c r="X38" s="25"/>
+      <c r="Y38" s="25"/>
+      <c r="Z38" s="25"/>
+      <c r="AA38" s="25"/>
       <c r="AB38" s="3"/>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
@@ -27385,22 +27413,22 @@
       <c r="H39" s="21"/>
       <c r="I39" s="21"/>
       <c r="J39" s="22"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="34"/>
-      <c r="S39" s="34"/>
-      <c r="T39" s="34"/>
-      <c r="U39" s="34"/>
-      <c r="V39" s="34"/>
-      <c r="W39" s="34"/>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
-      <c r="AA39" s="34"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+      <c r="T39" s="25"/>
+      <c r="U39" s="25"/>
+      <c r="V39" s="25"/>
+      <c r="W39" s="25"/>
+      <c r="X39" s="25"/>
+      <c r="Y39" s="25"/>
+      <c r="Z39" s="25"/>
+      <c r="AA39" s="25"/>
       <c r="AB39" s="3"/>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
@@ -27434,15 +27462,15 @@
       <c r="J40" s="13">
         <v>500000</v>
       </c>
-      <c r="L40" s="34"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
-      <c r="O40" s="34"/>
-      <c r="P40" s="34"/>
-      <c r="Q40" s="34"/>
-      <c r="R40" s="34"/>
-      <c r="S40" s="34"/>
-      <c r="T40" s="34"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="25"/>
+      <c r="S40" s="25"/>
+      <c r="T40" s="25"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
@@ -27689,10 +27717,10 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="36"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="7" t="s">
         <v>6</v>
       </c>
@@ -28223,8 +28251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7326F72D-FE2E-4499-9C3F-B7DCE9FC1F96}">
   <dimension ref="A1:U71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U9"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28233,18 +28261,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
       <c r="L1" s="5" t="s">
         <v>24</v>
       </c>
@@ -28253,10 +28281,10 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
@@ -28624,10 +28652,10 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="7" t="s">
         <v>6</v>
       </c>
@@ -28936,10 +28964,10 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="27"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="7" t="s">
         <v>6</v>
       </c>
@@ -29245,10 +29273,10 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="36"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="7" t="s">
         <v>6</v>
       </c>
@@ -29620,34 +29648,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
-      <c r="L1" s="32" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
+      <c r="L1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
@@ -29662,14 +29690,14 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
       <c r="U2" t="s">
         <v>32</v>
       </c>
@@ -29687,14 +29715,14 @@
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
       <c r="J3" s="22"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
       <c r="U3" t="s">
         <v>7</v>
       </c>
@@ -29733,14 +29761,14 @@
       <c r="J4" s="13">
         <v>500000</v>
       </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
       <c r="U4" t="s">
         <v>8</v>
       </c>
@@ -30084,10 +30112,10 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="7" t="s">
         <v>16</v>
       </c>
@@ -30451,10 +30479,10 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="27"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="7" t="s">
         <v>16</v>
       </c>
@@ -30841,10 +30869,10 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="36"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="7" t="s">
         <v>16</v>
       </c>
@@ -31250,18 +31278,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
       <c r="L1" s="5" t="s">
         <v>24</v>
       </c>
@@ -31270,10 +31298,10 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
@@ -31682,10 +31710,10 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="7" t="s">
         <v>16</v>
       </c>
@@ -32046,10 +32074,10 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="27"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="7" t="s">
         <v>16</v>
       </c>
@@ -32385,10 +32413,10 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="36"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="7" t="s">
         <v>16</v>
       </c>
@@ -32759,7 +32787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B84FEB5D-2983-4E4D-A643-6C81170FF3BE}">
   <dimension ref="A1:X71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
@@ -32769,34 +32797,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
-      <c r="L1" s="32" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
+      <c r="L1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
@@ -32811,14 +32839,14 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="8"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
       <c r="U2" t="s">
         <v>32</v>
       </c>
@@ -32836,14 +32864,14 @@
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
       <c r="J3" s="22"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
       <c r="U3" t="s">
         <v>7</v>
       </c>
@@ -32882,14 +32910,14 @@
       <c r="J4" s="13">
         <v>500000</v>
       </c>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
       <c r="U4" t="s">
         <v>8</v>
       </c>
@@ -33305,10 +33333,10 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="7" t="s">
         <v>18</v>
       </c>
@@ -33705,10 +33733,10 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="27"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="7" t="s">
         <v>18</v>
       </c>
@@ -34107,10 +34135,10 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="36"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="7" t="s">
         <v>18</v>
       </c>
@@ -34416,39 +34444,39 @@
         <v>3</v>
       </c>
       <c r="B69" s="1">
-        <f>AVERAGE(B59:B68)</f>
+        <f t="shared" ref="B69:H69" si="9">AVERAGE(B59:B68)</f>
         <v>65.3</v>
       </c>
       <c r="C69" s="1">
-        <f>AVERAGE(C59:C68)</f>
+        <f t="shared" si="9"/>
         <v>68</v>
       </c>
       <c r="D69" s="1">
-        <f>AVERAGE(D59:D68)</f>
+        <f t="shared" si="9"/>
         <v>99.666666666666671</v>
       </c>
       <c r="E69" s="1">
-        <f>AVERAGE(E59:E68)</f>
+        <f t="shared" si="9"/>
         <v>137.80000000000001</v>
       </c>
       <c r="F69" s="1">
-        <f>AVERAGE(F59:F68)</f>
+        <f t="shared" si="9"/>
         <v>382.75</v>
       </c>
       <c r="G69" s="1">
-        <f>AVERAGE(G59:G68)</f>
+        <f t="shared" si="9"/>
         <v>713.2</v>
       </c>
       <c r="H69" s="1">
-        <f>AVERAGE(H59:H68)</f>
+        <f t="shared" si="9"/>
         <v>3253.8</v>
       </c>
       <c r="I69" s="1" t="e">
-        <f t="shared" ref="I69:J69" si="9">AVERAGE(I59:I68)</f>
+        <f t="shared" ref="I69:J69" si="10">AVERAGE(I59:I68)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J69" s="13" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -34457,39 +34485,39 @@
         <v>4</v>
       </c>
       <c r="B70">
-        <f>_xlfn.STDEV.P(B59:B68)</f>
+        <f t="shared" ref="B70:H70" si="11">_xlfn.STDEV.P(B59:B68)</f>
         <v>5.3113086899558004</v>
       </c>
       <c r="C70">
-        <f>_xlfn.STDEV.P(C59:C68)</f>
+        <f t="shared" si="11"/>
         <v>6.6332495807107996</v>
       </c>
       <c r="D70">
-        <f>_xlfn.STDEV.P(D59:D68)</f>
+        <f t="shared" si="11"/>
         <v>5.5277079839256666</v>
       </c>
       <c r="E70">
-        <f>_xlfn.STDEV.P(E59:E68)</f>
+        <f t="shared" si="11"/>
         <v>8.2559069762201176</v>
       </c>
       <c r="F70">
-        <f>_xlfn.STDEV.P(F59:F68)</f>
+        <f t="shared" si="11"/>
         <v>1.479019945774904</v>
       </c>
       <c r="G70">
-        <f>_xlfn.STDEV.P(G59:G68)</f>
+        <f t="shared" si="11"/>
         <v>30.049292836937113</v>
       </c>
       <c r="H70">
-        <f>_xlfn.STDEV.P(H59:H68)</f>
+        <f t="shared" si="11"/>
         <v>28.784718167805639</v>
       </c>
       <c r="I70" t="e">
-        <f t="shared" ref="I70:J70" si="10">_xlfn.STDEV.P(I59:I68)</f>
+        <f t="shared" ref="I70:J70" si="12">_xlfn.STDEV.P(I59:I68)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J70" s="15" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -34498,54 +34526,54 @@
         <v>5</v>
       </c>
       <c r="B71" s="17">
-        <f>_xlfn.STDEV.S(B59:B68)</f>
+        <f t="shared" ref="B71:H71" si="13">_xlfn.STDEV.S(B59:B68)</f>
         <v>5.5986109388351357</v>
       </c>
       <c r="C71" s="17">
-        <f>_xlfn.STDEV.S(C59:C68)</f>
+        <f t="shared" si="13"/>
         <v>7.0912420834233467</v>
       </c>
       <c r="D71" s="17">
-        <f>_xlfn.STDEV.S(D59:D68)</f>
+        <f t="shared" si="13"/>
         <v>6.0553007081949835</v>
       </c>
       <c r="E71" s="17">
-        <f>_xlfn.STDEV.S(E59:E68)</f>
+        <f t="shared" si="13"/>
         <v>9.2303846073714606</v>
       </c>
       <c r="F71" s="17">
-        <f>_xlfn.STDEV.S(F59:F68)</f>
+        <f t="shared" si="13"/>
         <v>1.707825127659933</v>
       </c>
       <c r="G71" s="17">
-        <f>_xlfn.STDEV.S(G59:G68)</f>
+        <f t="shared" si="13"/>
         <v>33.596130729594442</v>
       </c>
       <c r="H71" s="17">
-        <f>_xlfn.STDEV.S(H59:H68)</f>
+        <f t="shared" si="13"/>
         <v>32.182293268193305</v>
       </c>
       <c r="I71" s="17" t="e">
-        <f t="shared" ref="I71:J71" si="11">_xlfn.STDEV.S(I59:I68)</f>
+        <f t="shared" ref="I71:J71" si="14">_xlfn.STDEV.S(I59:I68)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="J71" s="18" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="L1:S4"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B39:J39"/>
     <mergeCell ref="B57:J57"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="L1:S4"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="B39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -34567,18 +34595,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
       <c r="L1" s="5" t="s">
         <v>24</v>
       </c>
@@ -34587,10 +34615,10 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="31"/>
+      <c r="B2" s="36"/>
       <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
@@ -35044,10 +35072,10 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="7" t="s">
         <v>18</v>
       </c>
@@ -35429,10 +35457,10 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="27"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="7" t="s">
         <v>18</v>
       </c>
@@ -35804,10 +35832,10 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
+      <c r="A56" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="36"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="7" t="s">
         <v>18</v>
       </c>
@@ -36223,4 +36251,182 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1083D35-1455-4A6A-8D2F-88B4EAE334E1}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="1">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1">
+        <v>500</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>58</v>
+      </c>
+      <c r="E4">
+        <v>114</v>
+      </c>
+      <c r="F4">
+        <v>569</v>
+      </c>
+      <c r="G4">
+        <v>1138</v>
+      </c>
+      <c r="H4">
+        <v>5686</v>
+      </c>
+      <c r="I4">
+        <v>11371</v>
+      </c>
+      <c r="J4">
+        <v>56851</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>148</v>
+      </c>
+      <c r="E5">
+        <v>300</v>
+      </c>
+      <c r="F5">
+        <v>1554</v>
+      </c>
+      <c r="G5">
+        <v>3135</v>
+      </c>
+      <c r="H5">
+        <v>15631</v>
+      </c>
+      <c r="I5">
+        <v>31402</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>146</v>
+      </c>
+      <c r="E6">
+        <v>297</v>
+      </c>
+      <c r="F6">
+        <v>1467</v>
+      </c>
+      <c r="G6">
+        <v>2931</v>
+      </c>
+      <c r="H6">
+        <v>14740</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>